<commit_message>
Fixed libraries and import in VSCode
</commit_message>
<xml_diff>
--- a/Data/VALETUDO_database_1st_batch_en_all_info.xlsx
+++ b/Data/VALETUDO_database_1st_batch_en_all_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Il mio Drive\_DIDATTICA\_POLIMI\AI_Methods_BioEngineering\_2025-2026\04_ECG_Challenge\Source\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\PhD\courses\AI Methods for Bioengineering Challenges\challenge\ecg_challenge\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E042FC7D-3871-43A1-88BC-FCFFC4E63C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B50F2E3-855E-405E-8162-CE71F3782950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,7 +165,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A192"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>